<commit_message>
index and craftsman list
</commit_message>
<xml_diff>
--- a/doc/wxapp-plan.xlsx
+++ b/doc/wxapp-plan.xlsx
@@ -693,6 +693,24 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="12" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,24 +722,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="12" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
@@ -1384,7 +1384,7 @@
   <dimension ref="B1:BO34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
@@ -1412,13 +1412,13 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1426,66 +1426,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
       <c r="T2" s="10"/>
       <c r="U2" s="11"/>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
       <c r="Y2" s="10"/>
       <c r="Z2" s="12"/>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
       <c r="AF2" s="13"/>
       <c r="AG2" s="14"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AH2" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="31"/>
-      <c r="AL2" s="31"/>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
       <c r="AO2" s="15"/>
       <c r="AP2" s="15"/>
     </row>
     <row r="3" spans="2:67" s="19" customFormat="1" ht="40" customHeight="1" thickTop="1">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="16" t="s">
@@ -1512,12 +1512,12 @@
       <c r="AA3" s="18"/>
     </row>
     <row r="4" spans="2:67" ht="37" customHeight="1">
-      <c r="B4" s="38"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="20">
         <v>1</v>
       </c>
@@ -2117,6 +2117,11 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AN2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
@@ -2124,11 +2129,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="AH2:AN2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="BP5:BP7">

</xml_diff>

<commit_message>
order personal order-form style
</commit_message>
<xml_diff>
--- a/doc/wxapp-plan.xlsx
+++ b/doc/wxapp-plan.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>活动</t>
   </si>
@@ -125,10 +125,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>全部订单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>订单详情页面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -197,6 +193,14 @@
   </si>
   <si>
     <t xml:space="preserve">完成（超出计划）百分比 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全部订单页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全部订单页面功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -204,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -357,6 +361,22 @@
       <sz val="18"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Microsoft YaHei UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -534,7 +554,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,6 +623,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -693,6 +719,18 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -711,20 +749,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="26">
     <cellStyle name="百分比" xfId="23" builtinId="5"/>
     <cellStyle name="标签" xfId="5"/>
     <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
@@ -732,6 +758,8 @@
     <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="超链接" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="汇总" xfId="22" builtinId="25" customBuiltin="1"/>
     <cellStyle name="活动" xfId="2"/>
     <cellStyle name="计划图例" xfId="14"/>
@@ -1381,10 +1409,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO34"/>
+  <dimension ref="B1:BO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
@@ -1412,13 +1440,13 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1426,66 +1454,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
       <c r="N2" s="8"/>
       <c r="O2" s="9"/>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
       <c r="T2" s="10"/>
       <c r="U2" s="11"/>
-      <c r="V2" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
+      <c r="V2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
       <c r="Y2" s="10"/>
       <c r="Z2" s="12"/>
-      <c r="AA2" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
+      <c r="AA2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="13"/>
       <c r="AG2" s="14"/>
-      <c r="AH2" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
+      <c r="AH2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
       <c r="AO2" s="15"/>
       <c r="AP2" s="15"/>
     </row>
     <row r="3" spans="2:67" s="19" customFormat="1" ht="40" customHeight="1" thickTop="1">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="34" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="16" t="s">
@@ -1512,12 +1540,12 @@
       <c r="AA3" s="18"/>
     </row>
     <row r="4" spans="2:67" ht="37" customHeight="1">
-      <c r="B4" s="34"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="20">
         <v>1</v>
       </c>
@@ -1915,7 +1943,12 @@
       <c r="E14" s="3">
         <v>9</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="F14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="2:67" ht="62" customHeight="1">
       <c r="B15" s="21" t="s">
@@ -1927,35 +1960,59 @@
       <c r="D15" s="3">
         <v>0.5</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="E15" s="3">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:67" ht="62" customHeight="1">
       <c r="B16" s="21" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3">
         <v>10</v>
       </c>
       <c r="D16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="3">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="29">
         <v>1</v>
       </c>
-      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" ht="62" customHeight="1">
       <c r="B17" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3">
         <v>0.8</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="E17" s="3">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="62" customHeight="1">
       <c r="B18" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3">
         <v>11</v>
@@ -1967,10 +2024,10 @@
     </row>
     <row r="19" spans="2:7" ht="62" customHeight="1">
       <c r="B19" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="3">
         <v>0.5</v>
@@ -1979,7 +2036,7 @@
     </row>
     <row r="20" spans="2:7" ht="62" customHeight="1">
       <c r="B20" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
@@ -1987,14 +2044,22 @@
       <c r="D20" s="3">
         <v>0.5</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="E20" s="3">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:7" ht="62" customHeight="1">
       <c r="B21" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="3">
         <v>0.5</v>
@@ -2003,7 +2068,7 @@
     </row>
     <row r="22" spans="2:7" ht="62" customHeight="1">
       <c r="B22" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3">
         <v>13</v>
@@ -2015,10 +2080,10 @@
     </row>
     <row r="23" spans="2:7" ht="62" customHeight="1">
       <c r="B23" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3">
         <v>0.3</v>
@@ -2027,10 +2092,10 @@
     </row>
     <row r="24" spans="2:7" ht="62" customHeight="1">
       <c r="B24" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3">
         <v>0.2</v>
@@ -2039,7 +2104,7 @@
     </row>
     <row r="25" spans="2:7" ht="62" customHeight="1">
       <c r="B25" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3">
         <v>16</v>
@@ -2051,7 +2116,7 @@
     </row>
     <row r="26" spans="2:7" ht="62" customHeight="1">
       <c r="B26" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3">
         <v>16</v>
@@ -2063,10 +2128,10 @@
     </row>
     <row r="27" spans="2:7" ht="62" customHeight="1">
       <c r="B27" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3">
         <v>0.7</v>
@@ -2075,7 +2140,7 @@
     </row>
     <row r="28" spans="2:7" ht="62" customHeight="1">
       <c r="B28" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3">
         <v>17</v>
@@ -2087,7 +2152,7 @@
     </row>
     <row r="29" spans="2:7" ht="62" customHeight="1">
       <c r="B29" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="3">
         <v>19</v>
@@ -2111,7 +2176,7 @@
     </row>
     <row r="31" spans="2:7" ht="62" customHeight="1">
       <c r="B31" s="21" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C31" s="3">
         <v>23</v>
@@ -2123,10 +2188,10 @@
     </row>
     <row r="32" spans="2:7" ht="62" customHeight="1">
       <c r="B32" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D32" s="3">
         <v>0.5</v>
@@ -2135,36 +2200,43 @@
     </row>
     <row r="33" spans="2:7" ht="62" customHeight="1">
       <c r="B33" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3">
         <v>24</v>
       </c>
       <c r="D33" s="3">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G33" s="29"/>
     </row>
     <row r="34" spans="2:7" ht="62" customHeight="1">
       <c r="B34" s="21" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C34" s="3">
         <v>24</v>
       </c>
       <c r="D34" s="3">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G34" s="29"/>
+    </row>
+    <row r="35" spans="2:7" ht="62" customHeight="1">
+      <c r="B35" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="3">
+        <v>24</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="29"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="12">
-    <mergeCell ref="AH2:AN2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="K2:M2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
@@ -2172,6 +2244,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="AH2:AN2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="BP5:BP7">
@@ -2200,7 +2277,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:BO34 H5:M7">
+  <conditionalFormatting sqref="H8:BO35 H5:M7">
     <cfRule type="expression" dxfId="19" priority="4">
       <formula>完成百分比</formula>
     </cfRule>
@@ -2257,17 +2334,17 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
+  <conditionalFormatting sqref="B33">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C33">
+  <conditionalFormatting sqref="C33:C34">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32:D33">
+  <conditionalFormatting sqref="D33:D34">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>